<commit_message>
add detailed table results
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdullah/Development/cpp/why-compiled-langs/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912D1385-2A06-CF4B-AA42-4EAECA5BF194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14CA058-B40C-064A-B3DF-357BA5FDD0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{CDBB9EFB-DB80-5041-BD6B-73FA57D8E5F0}"/>
   </bookViews>
@@ -2210,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB49E93-215A-8643-98BA-49146078E219}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add javascript (Node) experiment
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdullah/Development/cpp/why-compiled-langs/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14CA058-B40C-064A-B3DF-357BA5FDD0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAA737D-8191-EA41-842C-4F525413F4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{CDBB9EFB-DB80-5041-BD6B-73FA57D8E5F0}"/>
   </bookViews>
@@ -259,9 +259,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>C++</c:v>
                 </c:pt>
@@ -276,16 +276,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JavaScript</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
@@ -300,6 +303,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>17.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,9 +565,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>C++</c:v>
                 </c:pt>
@@ -576,16 +582,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JavaScript</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Sheet1!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>7.49</c:v>
                 </c:pt>
@@ -600,6 +609,9 @@
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>4.66</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>22.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2210,8 +2222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB49E93-215A-8643-98BA-49146078E219}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2291,8 +2303,12 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="1">
+        <v>0.873</v>
+      </c>
+      <c r="C7" s="1">
+        <v>22.97</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>